<commit_message>
home work at 8/27
</commit_message>
<xml_diff>
--- a/ScreenTransitionDiagram.xlsx
+++ b/ScreenTransitionDiagram.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayuki.shino/training/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukku\training\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -117,8 +117,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -166,13 +166,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -183,6 +183,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -204,7 +207,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="正方形/長方形 6"/>
+        <xdr:cNvPr id="7" name="正方形/長方形 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -293,7 +302,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="正方形/長方形 7"/>
+        <xdr:cNvPr id="8" name="正方形/長方形 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -382,7 +397,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="正方形/長方形 8"/>
+        <xdr:cNvPr id="9" name="正方形/長方形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -471,7 +492,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="正方形/長方形 10"/>
+        <xdr:cNvPr id="11" name="正方形/長方形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -560,7 +587,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="正方形/長方形 11"/>
+        <xdr:cNvPr id="12" name="正方形/長方形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -649,7 +682,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+        <xdr:cNvPr id="13" name="正方形/長方形 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -722,7 +761,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="正方形/長方形 13"/>
+        <xdr:cNvPr id="14" name="正方形/長方形 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -811,7 +856,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="正方形/長方形 14"/>
+        <xdr:cNvPr id="15" name="正方形/長方形 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -900,7 +951,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="正方形/長方形 19"/>
+        <xdr:cNvPr id="20" name="正方形/長方形 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -989,7 +1046,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="正方形/長方形 20"/>
+        <xdr:cNvPr id="21" name="正方形/長方形 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1078,7 +1141,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="直線矢印コネクタ 25"/>
+        <xdr:cNvPr id="26" name="直線矢印コネクタ 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="20" idx="3"/>
           <a:endCxn id="21" idx="1"/>
@@ -1128,7 +1197,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="直線矢印コネクタ 28"/>
+        <xdr:cNvPr id="29" name="直線矢印コネクタ 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="21" idx="3"/>
           <a:endCxn id="36" idx="1"/>
@@ -1178,7 +1253,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="直線矢印コネクタ 29"/>
+        <xdr:cNvPr id="30" name="直線矢印コネクタ 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="36" idx="3"/>
           <a:endCxn id="7" idx="1"/>
@@ -1228,7 +1309,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="正方形/長方形 35"/>
+        <xdr:cNvPr id="36" name="正方形/長方形 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1317,7 +1404,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="41" name="直線矢印コネクタ 40"/>
+        <xdr:cNvPr id="41" name="直線矢印コネクタ 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="21" idx="2"/>
           <a:endCxn id="8" idx="0"/>
@@ -1367,7 +1460,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="42" name="直線矢印コネクタ 41"/>
+        <xdr:cNvPr id="42" name="直線矢印コネクタ 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="8" idx="2"/>
           <a:endCxn id="11" idx="0"/>
@@ -1417,7 +1516,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="48" name="カギ線コネクタ 47"/>
+        <xdr:cNvPr id="48" name="カギ線コネクタ 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="36" idx="2"/>
           <a:endCxn id="9" idx="0"/>
@@ -1469,7 +1574,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="55" name="カギ線コネクタ 54"/>
+        <xdr:cNvPr id="55" name="カギ線コネクタ 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="21" idx="0"/>
           <a:endCxn id="20" idx="0"/>
@@ -1521,7 +1632,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="59" name="カギ線コネクタ 58"/>
+        <xdr:cNvPr id="59" name="カギ線コネクタ 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="9" idx="3"/>
           <a:endCxn id="12" idx="1"/>
@@ -1573,7 +1690,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="63" name="カギ線コネクタ 62"/>
+        <xdr:cNvPr id="63" name="カギ線コネクタ 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="9" idx="3"/>
           <a:endCxn id="14" idx="1"/>
@@ -1625,7 +1748,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="68" name="直線矢印コネクタ 67"/>
+        <xdr:cNvPr id="68" name="直線矢印コネクタ 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="9" idx="3"/>
           <a:endCxn id="13" idx="1"/>
@@ -1675,7 +1804,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="71" name="直線矢印コネクタ 70"/>
+        <xdr:cNvPr id="71" name="直線矢印コネクタ 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="12" idx="3"/>
           <a:endCxn id="15" idx="1"/>
@@ -1725,7 +1860,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="カギ線コネクタ 85"/>
+        <xdr:cNvPr id="86" name="カギ線コネクタ 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="7" idx="2"/>
           <a:endCxn id="9" idx="0"/>
@@ -1777,7 +1918,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="93" name="正方形/長方形 92"/>
+        <xdr:cNvPr id="93" name="正方形/長方形 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1850,7 +1997,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="94" name="正方形/長方形 93"/>
+        <xdr:cNvPr id="94" name="正方形/長方形 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1923,7 +2076,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="95" name="カギ線コネクタ 94"/>
+        <xdr:cNvPr id="95" name="カギ線コネクタ 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="13" idx="3"/>
           <a:endCxn id="93" idx="1"/>
@@ -1975,7 +2134,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="99" name="カギ線コネクタ 98"/>
+        <xdr:cNvPr id="99" name="カギ線コネクタ 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="13" idx="3"/>
           <a:endCxn id="94" idx="1"/>
@@ -2027,7 +2192,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="102" name="正方形/長方形 101"/>
+        <xdr:cNvPr id="102" name="正方形/長方形 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000066000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2100,7 +2271,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="103" name="正方形/長方形 102"/>
+        <xdr:cNvPr id="103" name="正方形/長方形 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000067000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2173,7 +2350,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="104" name="直線矢印コネクタ 103"/>
+        <xdr:cNvPr id="104" name="直線矢印コネクタ 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000068000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="93" idx="3"/>
           <a:endCxn id="102" idx="1"/>
@@ -2223,7 +2406,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="105" name="直線矢印コネクタ 104"/>
+        <xdr:cNvPr id="105" name="直線矢印コネクタ 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000069000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="94" idx="3"/>
           <a:endCxn id="103" idx="1"/>
@@ -2273,7 +2462,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="110" name="正方形/長方形 109"/>
+        <xdr:cNvPr id="110" name="正方形/長方形 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2400,7 +2595,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="111" name="正方形/長方形 110"/>
+        <xdr:cNvPr id="111" name="正方形/長方形 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2489,7 +2690,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="112" name="正方形/長方形 111"/>
+        <xdr:cNvPr id="112" name="正方形/長方形 111">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000070000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2578,7 +2785,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="113" name="正方形/長方形 112"/>
+        <xdr:cNvPr id="113" name="正方形/長方形 112">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000071000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2667,7 +2880,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="114" name="正方形/長方形 113"/>
+        <xdr:cNvPr id="114" name="正方形/長方形 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2756,7 +2975,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="115" name="正方形/長方形 114"/>
+        <xdr:cNvPr id="115" name="正方形/長方形 114">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000073000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2845,7 +3070,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="116" name="正方形/長方形 115"/>
+        <xdr:cNvPr id="116" name="正方形/長方形 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000074000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2934,7 +3165,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="117" name="正方形/長方形 116"/>
+        <xdr:cNvPr id="117" name="正方形/長方形 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3023,7 +3260,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="118" name="正方形/長方形 117"/>
+        <xdr:cNvPr id="118" name="正方形/長方形 117">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000076000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3112,7 +3355,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="119" name="正方形/長方形 118"/>
+        <xdr:cNvPr id="119" name="正方形/長方形 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000077000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3184,6 +3433,344 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1112157</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="直線矢印コネクタ 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E048BFE-642B-408E-9A96-F95CC80D26AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="3"/>
+          <a:endCxn id="116" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22368782" y="11576050"/>
+          <a:ext cx="2316843" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="直線矢印コネクタ 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37E1D953-5AE4-4D1E-B6BA-43CDE3C22899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="116" idx="3"/>
+          <a:endCxn id="118" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26940781" y="11576050"/>
+          <a:ext cx="2316844" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="直線矢印コネクタ 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23F8749-17D9-40FC-A530-B4FC55C9BCA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="117" idx="3"/>
+          <a:endCxn id="119" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26940781" y="14624050"/>
+          <a:ext cx="2316844" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1112157</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="カギ線コネクタ 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EBB9A63-2A0C-4FDB-8A1A-623DC9289433}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="3"/>
+          <a:endCxn id="117" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22368782" y="11576050"/>
+          <a:ext cx="2316843" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1127579</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1128713</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="直線矢印コネクタ 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0029736-4CC3-4BDD-9F17-458E2B05BEC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+          <a:endCxn id="110" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13240204" y="8166100"/>
+          <a:ext cx="1134" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1127579</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1127579</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="直線矢印コネクタ 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8098FF82-42BA-4FA4-BBE6-730F5E46F03F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="110" idx="2"/>
+          <a:endCxn id="111" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13240204" y="12738100"/>
+          <a:ext cx="0" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3454,122 +4041,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AC60" sqref="AC60"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="19.5"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="4:22" x14ac:dyDescent="0.3">
-      <c r="D2" s="2" t="s">
+    <row r="2" spans="4:22">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
-    <row r="9" spans="4:22" x14ac:dyDescent="0.3">
-      <c r="D9" s="2" t="s">
+    <row r="9" spans="4:22">
+      <c r="D9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="E9" s="3"/>
+      <c r="H9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="L9" s="2" t="s">
+      <c r="I9" s="3"/>
+      <c r="L9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="Q9" s="2" t="s">
+      <c r="M9" s="3"/>
+      <c r="Q9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R9" s="2"/>
-      <c r="U9" s="2" t="s">
+      <c r="R9" s="3"/>
+      <c r="U9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V9" s="2"/>
+      <c r="V9" s="3"/>
     </row>
-    <row r="18" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="L18" s="2" t="s">
+    <row r="18" spans="5:26">
+      <c r="L18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M18" s="2"/>
+      <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E19" s="2" t="s">
+    <row r="19" spans="5:26">
+      <c r="E19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+      <c r="F19" s="3"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
     </row>
-    <row r="21" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="U21" s="1" t="s">
+    <row r="21" spans="5:26">
+      <c r="U21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V21" s="1"/>
-      <c r="Y21" s="1" t="s">
+      <c r="V21" s="2"/>
+      <c r="Y21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Z21" s="1"/>
+      <c r="Z21" s="2"/>
     </row>
-    <row r="27" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="Q27" s="1" t="s">
+    <row r="27" spans="5:26">
+      <c r="Q27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R27" s="1"/>
+      <c r="R27" s="2"/>
     </row>
-    <row r="35" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="U35" s="1" t="s">
+    <row r="35" spans="5:26">
+      <c r="U35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V35" s="1"/>
-      <c r="Y35" s="1" t="s">
+      <c r="V35" s="2"/>
+      <c r="Y35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Z35" s="1"/>
+      <c r="Z35" s="2"/>
     </row>
-    <row r="37" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E37" s="2" t="s">
+    <row r="37" spans="5:26">
+      <c r="E37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="2"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
     </row>
-    <row r="39" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
+    <row r="39" spans="5:26">
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
     </row>
-    <row r="45" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="Q45" s="1" t="s">
+    <row r="45" spans="5:26">
+      <c r="Q45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R45" s="1"/>
+      <c r="R45" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Y35:Z35"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="K19:N19"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y35:Z35"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit 8/28 add SDD
</commit_message>
<xml_diff>
--- a/ScreenTransitionDiagram.xlsx
+++ b/ScreenTransitionDiagram.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukku\training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayuki.shino/training/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,98 +27,173 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>ログイン</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>間違い</t>
     <rPh sb="0" eb="2">
       <t>マチガ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>検索</t>
     <rPh sb="0" eb="2">
       <t>ケンサk</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ソート</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>店舗登録ボタン</t>
     <rPh sb="0" eb="4">
       <t>テンp</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>店舗選択</t>
     <rPh sb="0" eb="4">
       <t>テンp</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>登録</t>
     <rPh sb="0" eb="2">
       <t>トウロk</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>更新</t>
     <rPh sb="0" eb="2">
       <t>コウシn</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>メニュー登録</t>
     <rPh sb="4" eb="6">
       <t>トウロk</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>メニュー一覧</t>
     <rPh sb="4" eb="6">
       <t>イチラn</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>店舗情報編集ボタン</t>
     <rPh sb="0" eb="6">
       <t>テンp</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>メニュー編集</t>
     <rPh sb="4" eb="6">
       <t>ヘンシュ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>評価一覧</t>
     <rPh sb="0" eb="4">
       <t>ヒョ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シーン選択</t>
+    <rPh sb="3" eb="5">
+      <t>センタk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>写真登録ボタン</t>
+    <rPh sb="0" eb="2">
+      <t>シャシn</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>トウロk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>写真編集ボタン</t>
+    <rPh sb="0" eb="2">
+      <t>シャシn</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ヘンシュ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>評価登録ボタン</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョウk</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>トウロk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>評価編集</t>
+    <rPh sb="0" eb="4">
+      <t>ヒョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>評価一覧</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>イチラn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パスワード変更</t>
+    <rPh sb="5" eb="7">
+      <t>ヘンコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メールアドレス入力</t>
+    <rPh sb="7" eb="9">
+      <t>ニュウry</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>写真一覧</t>
+    <rPh sb="0" eb="4">
+      <t>シャシn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,8 +203,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="6"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
@@ -137,7 +219,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
       <charset val="128"/>
@@ -164,14 +248,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -210,7 +300,7 @@
         <xdr:cNvPr id="7" name="正方形/長方形 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -305,7 +395,7 @@
         <xdr:cNvPr id="8" name="正方形/長方形 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -400,7 +490,7 @@
         <xdr:cNvPr id="9" name="正方形/長方形 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -495,7 +585,7 @@
         <xdr:cNvPr id="11" name="正方形/長方形 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -590,7 +680,7 @@
         <xdr:cNvPr id="12" name="正方形/長方形 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -685,7 +775,7 @@
         <xdr:cNvPr id="13" name="正方形/長方形 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -764,7 +854,7 @@
         <xdr:cNvPr id="14" name="正方形/長方形 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -859,7 +949,7 @@
         <xdr:cNvPr id="15" name="正方形/長方形 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -954,7 +1044,7 @@
         <xdr:cNvPr id="20" name="正方形/長方形 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1049,7 +1139,7 @@
         <xdr:cNvPr id="21" name="正方形/長方形 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1144,7 +1234,7 @@
         <xdr:cNvPr id="26" name="直線矢印コネクタ 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1200,7 +1290,7 @@
         <xdr:cNvPr id="29" name="直線矢印コネクタ 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1256,7 +1346,7 @@
         <xdr:cNvPr id="30" name="直線矢印コネクタ 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1312,7 +1402,7 @@
         <xdr:cNvPr id="36" name="正方形/長方形 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1407,7 +1497,7 @@
         <xdr:cNvPr id="41" name="直線矢印コネクタ 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1463,7 +1553,7 @@
         <xdr:cNvPr id="42" name="直線矢印コネクタ 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1519,7 +1609,7 @@
         <xdr:cNvPr id="48" name="カギ線コネクタ 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1577,7 +1667,7 @@
         <xdr:cNvPr id="55" name="カギ線コネクタ 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000037000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1635,7 +1725,7 @@
         <xdr:cNvPr id="59" name="カギ線コネクタ 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1693,7 +1783,7 @@
         <xdr:cNvPr id="63" name="カギ線コネクタ 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1751,7 +1841,7 @@
         <xdr:cNvPr id="68" name="直線矢印コネクタ 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000044000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1807,7 +1897,7 @@
         <xdr:cNvPr id="71" name="直線矢印コネクタ 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000047000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1863,7 +1953,7 @@
         <xdr:cNvPr id="86" name="カギ線コネクタ 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000056000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1921,7 +2011,7 @@
         <xdr:cNvPr id="93" name="正方形/長方形 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2000,7 +2090,7 @@
         <xdr:cNvPr id="94" name="正方形/長方形 93">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2079,7 +2169,7 @@
         <xdr:cNvPr id="95" name="カギ線コネクタ 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00005F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2137,7 +2227,7 @@
         <xdr:cNvPr id="99" name="カギ線コネクタ 98">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000063000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2195,7 +2285,7 @@
         <xdr:cNvPr id="102" name="正方形/長方形 101">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000066000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000066000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2274,7 +2364,7 @@
         <xdr:cNvPr id="103" name="正方形/長方形 102">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000067000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000067000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2353,7 +2443,7 @@
         <xdr:cNvPr id="104" name="直線矢印コネクタ 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000068000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000068000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2409,7 +2499,7 @@
         <xdr:cNvPr id="105" name="直線矢印コネクタ 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000069000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000069000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2449,23 +2539,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1112157</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="110" name="正方形/長方形 109">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
+        <xdr:cNvPr id="116" name="正方形/長方形 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000074000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2473,7 +2563,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12340167" y="10414000"/>
+          <a:off x="24680333" y="10414000"/>
           <a:ext cx="2233990" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2519,45 +2609,7 @@
               <a:ea typeface="Meiryo" charset="-128"/>
               <a:cs typeface="Meiryo" charset="-128"/>
             </a:rPr>
-            <a:t>シーン</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
-            <a:ln w="0"/>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
-                <a:schemeClr val="dk1">
-                  <a:alpha val="40000"/>
-                </a:schemeClr>
-              </a:outerShdw>
-            </a:effectLst>
-            <a:latin typeface="Meiryo" charset="-128"/>
-            <a:ea typeface="Meiryo" charset="-128"/>
-            <a:cs typeface="Meiryo" charset="-128"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
-              <a:ln w="0"/>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:schemeClr val="dk1">
-                    <a:alpha val="40000"/>
-                  </a:schemeClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="Meiryo" charset="-128"/>
-              <a:ea typeface="Meiryo" charset="-128"/>
-              <a:cs typeface="Meiryo" charset="-128"/>
-            </a:rPr>
-            <a:t>一覧</a:t>
+            <a:t>評価入力</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" cap="none" spc="0">
             <a:ln w="0"/>
@@ -2582,23 +2634,645 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="117" name="正方形/長方形 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000075000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24680333" y="13462000"/>
+          <a:ext cx="2233990" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Meiryo" charset="-128"/>
+              <a:ea typeface="Meiryo" charset="-128"/>
+              <a:cs typeface="Meiryo" charset="-128"/>
+            </a:rPr>
+            <a:t>評価入力</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Meiryo" charset="-128"/>
+            <a:ea typeface="Meiryo" charset="-128"/>
+            <a:cs typeface="Meiryo" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>1112157</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="118" name="正方形/長方形 117">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000076000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="29167667" y="10414000"/>
+          <a:ext cx="2233990" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Meiryo" charset="-128"/>
+              <a:ea typeface="Meiryo" charset="-128"/>
+              <a:cs typeface="Meiryo" charset="-128"/>
+            </a:rPr>
+            <a:t>登録完了</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Meiryo" charset="-128"/>
+            <a:ea typeface="Meiryo" charset="-128"/>
+            <a:cs typeface="Meiryo" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>1112157</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="正方形/長方形 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000077000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="29167667" y="13462000"/>
+          <a:ext cx="2233990" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Meiryo" charset="-128"/>
+              <a:ea typeface="Meiryo" charset="-128"/>
+              <a:cs typeface="Meiryo" charset="-128"/>
+            </a:rPr>
+            <a:t>編集完了</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Meiryo" charset="-128"/>
+            <a:ea typeface="Meiryo" charset="-128"/>
+            <a:cs typeface="Meiryo" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1112157</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="直線矢印コネクタ 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2E048BFE-642B-408E-9A96-F95CC80D26AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="3"/>
+          <a:endCxn id="116" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22368782" y="11576050"/>
+          <a:ext cx="2316843" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="直線矢印コネクタ 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{37E1D953-5AE4-4D1E-B6BA-43CDE3C22899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="116" idx="3"/>
+          <a:endCxn id="118" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26940781" y="11576050"/>
+          <a:ext cx="2316844" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="直線矢印コネクタ 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E23F8749-17D9-40FC-A530-B4FC55C9BCA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="117" idx="3"/>
+          <a:endCxn id="119" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26940781" y="14624050"/>
+          <a:ext cx="2316844" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1112157</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="カギ線コネクタ 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2EBB9A63-2A0C-4FDB-8A1A-623DC9289433}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="3"/>
+          <a:endCxn id="117" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22368782" y="11576050"/>
+          <a:ext cx="2316843" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1127579</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1128713</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="直線矢印コネクタ 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B0029736-4CC3-4BDD-9F17-458E2B05BEC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13240204" y="8166100"/>
+          <a:ext cx="1134" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1143453</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1143453</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="直線矢印コネクタ 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8098FF82-42BA-4FA4-BBE6-730F5E46F03F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="61" idx="2"/>
+          <a:endCxn id="65" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15938953" y="17310100"/>
+          <a:ext cx="0" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1112157</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="111" name="正方形/長方形 110">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
+        <xdr:cNvPr id="50" name="正方形/長方形 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2606,8 +3280,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12340167" y="14986000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="12446000" y="10414000"/>
+          <a:ext cx="2286907" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2679,21 +3353,21 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1112157</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="112" name="正方形/長方形 111">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000070000000}"/>
+        <xdr:cNvPr id="60" name="正方形/長方形 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000070000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2701,8 +3375,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10096500" y="19558000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="10096500" y="14986000"/>
+          <a:ext cx="2286907" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2774,21 +3448,21 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>1112156</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="113" name="正方形/長方形 112">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000071000000}"/>
+        <xdr:cNvPr id="61" name="正方形/長方形 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000071000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2796,8 +3470,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14583833" y="19558000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="14795500" y="14986000"/>
+          <a:ext cx="2286906" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2869,21 +3543,21 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1112157</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="114" name="正方形/長方形 113">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+        <xdr:cNvPr id="64" name="正方形/長方形 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000072000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2891,8 +3565,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10096500" y="24130000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="10096500" y="19558000"/>
+          <a:ext cx="2286907" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2964,21 +3638,21 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>1112156</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="115" name="正方形/長方形 114">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000073000000}"/>
+        <xdr:cNvPr id="65" name="正方形/長方形 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000073000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2986,8 +3660,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14583833" y="24130000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="14795500" y="19558000"/>
+          <a:ext cx="2286906" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3057,23 +3731,195 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1143454</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1143454</xdr:colOff>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>1112156</xdr:colOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="直線矢印コネクタ 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8098FF82-42BA-4FA4-BBE6-730F5E46F03F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="60" idx="2"/>
+          <a:endCxn id="64" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11239954" y="17310100"/>
+          <a:ext cx="0" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1143453</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1143452</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="カギ線コネクタ 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="2"/>
+          <a:endCxn id="61" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="13640253" y="12687300"/>
+          <a:ext cx="2247900" cy="2349499"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1143454</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1143454</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="70" name="カギ線コネクタ 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="2"/>
+          <a:endCxn id="60" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="11290754" y="12687300"/>
+          <a:ext cx="2247900" cy="2349500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="116" name="正方形/長方形 115">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000074000000}"/>
+        <xdr:cNvPr id="73" name="正方形/長方形 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000073000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3081,8 +3927,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24680333" y="10414000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="21005800" y="17272000"/>
+          <a:ext cx="2305956" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3127,7 +3973,45 @@
               <a:ea typeface="Meiryo" charset="-128"/>
               <a:cs typeface="Meiryo" charset="-128"/>
             </a:rPr>
-            <a:t>評価入力</a:t>
+            <a:t>マイ</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Meiryo" charset="-128"/>
+            <a:ea typeface="Meiryo" charset="-128"/>
+            <a:cs typeface="Meiryo" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Meiryo" charset="-128"/>
+              <a:ea typeface="Meiryo" charset="-128"/>
+              <a:cs typeface="Meiryo" charset="-128"/>
+            </a:rPr>
+            <a:t>ページ</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" cap="none" spc="0">
             <a:ln w="0"/>
@@ -3154,21 +4038,21 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>1112156</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="117" name="正方形/長方形 116">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
+        <xdr:cNvPr id="74" name="正方形/長方形 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000073000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3176,8 +4060,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24680333" y="13462000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="25781000" y="17272000"/>
+          <a:ext cx="2305956" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3222,9 +4106,47 @@
               <a:ea typeface="Meiryo" charset="-128"/>
               <a:cs typeface="Meiryo" charset="-128"/>
             </a:rPr>
-            <a:t>評価入力</a:t>
+            <a:t>自分の</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" cap="none" spc="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Meiryo" charset="-128"/>
+            <a:ea typeface="Meiryo" charset="-128"/>
+            <a:cs typeface="Meiryo" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Meiryo" charset="-128"/>
+              <a:ea typeface="Meiryo" charset="-128"/>
+              <a:cs typeface="Meiryo" charset="-128"/>
+            </a:rPr>
+            <a:t>評価一覧</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
             <a:ln w="0"/>
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -3247,23 +4169,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>1112157</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="118" name="正方形/長方形 117">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000076000000}"/>
+        <xdr:cNvPr id="75" name="正方形/長方形 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000073000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3271,8 +4193,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29167667" y="10414000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="25781000" y="21844000"/>
+          <a:ext cx="2305956" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3317,9 +4239,47 @@
               <a:ea typeface="Meiryo" charset="-128"/>
               <a:cs typeface="Meiryo" charset="-128"/>
             </a:rPr>
-            <a:t>登録完了</a:t>
+            <a:t>自分の</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" cap="none" spc="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Meiryo" charset="-128"/>
+            <a:ea typeface="Meiryo" charset="-128"/>
+            <a:cs typeface="Meiryo" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Meiryo" charset="-128"/>
+              <a:ea typeface="Meiryo" charset="-128"/>
+              <a:cs typeface="Meiryo" charset="-128"/>
+            </a:rPr>
+            <a:t>写真一覧</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
             <a:ln w="0"/>
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -3342,23 +4302,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>1112157</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="119" name="正方形/長方形 118">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000077000000}"/>
+        <xdr:cNvPr id="76" name="正方形/長方形 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000073000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3366,8 +4326,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29167667" y="13462000"/>
-          <a:ext cx="2233990" cy="2324100"/>
+          <a:off x="21005800" y="21844000"/>
+          <a:ext cx="2305956" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3412,9 +4372,9 @@
               <a:ea typeface="Meiryo" charset="-128"/>
               <a:cs typeface="Meiryo" charset="-128"/>
             </a:rPr>
-            <a:t>編集完了</a:t>
+            <a:t>入力</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" cap="none" spc="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
             <a:ln w="0"/>
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -3437,35 +4397,168 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1112157</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="正方形/長方形 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000073000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21005800" y="26416000"/>
+          <a:ext cx="2305956" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Meiryo" charset="-128"/>
+              <a:ea typeface="Meiryo" charset="-128"/>
+              <a:cs typeface="Meiryo" charset="-128"/>
+            </a:rPr>
+            <a:t>メール</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Meiryo" charset="-128"/>
+            <a:ea typeface="Meiryo" charset="-128"/>
+            <a:cs typeface="Meiryo" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Meiryo" charset="-128"/>
+              <a:ea typeface="Meiryo" charset="-128"/>
+              <a:cs typeface="Meiryo" charset="-128"/>
+            </a:rPr>
+            <a:t>送信完了</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:latin typeface="Meiryo" charset="-128"/>
+            <a:ea typeface="Meiryo" charset="-128"/>
+            <a:cs typeface="Meiryo" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="49" name="直線矢印コネクタ 48">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E048BFE-642B-408E-9A96-F95CC80D26AF}"/>
+        <xdr:cNvPr id="81" name="直線矢印コネクタ 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E23F8749-17D9-40FC-A530-B4FC55C9BCA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="14" idx="3"/>
-          <a:endCxn id="116" idx="1"/>
+          <a:stCxn id="73" idx="3"/>
+          <a:endCxn id="74" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22368782" y="11576050"/>
-          <a:ext cx="2316843" cy="0"/>
+          <a:off x="23311756" y="18434050"/>
+          <a:ext cx="2469244" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3493,35 +4586,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>1112156</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1152978</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1152978</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="直線矢印コネクタ 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37E1D953-5AE4-4D1E-B6BA-43CDE3C22899}"/>
+        <xdr:cNvPr id="84" name="直線矢印コネクタ 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E23F8749-17D9-40FC-A530-B4FC55C9BCA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="116" idx="3"/>
-          <a:endCxn id="118" idx="1"/>
+          <a:stCxn id="73" idx="2"/>
+          <a:endCxn id="76" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="26940781" y="11576050"/>
-          <a:ext cx="2316844" cy="0"/>
+          <a:off x="22158778" y="19596100"/>
+          <a:ext cx="0" cy="2247900"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3549,35 +4642,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>1112156</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1152978</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1152978</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="54" name="直線矢印コネクタ 53">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23F8749-17D9-40FC-A530-B4FC55C9BCA9}"/>
+        <xdr:cNvPr id="85" name="直線矢印コネクタ 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E23F8749-17D9-40FC-A530-B4FC55C9BCA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="117" idx="3"/>
-          <a:endCxn id="119" idx="1"/>
+          <a:stCxn id="76" idx="2"/>
+          <a:endCxn id="79" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="26940781" y="14624050"/>
-          <a:ext cx="2316844" cy="0"/>
+          <a:off x="22158778" y="24168100"/>
+          <a:ext cx="0" cy="2247900"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3606,151 +4699,39 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1112157</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:colOff>1112156</xdr:colOff>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="58" name="カギ線コネクタ 98">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EBB9A63-2A0C-4FDB-8A1A-623DC9289433}"/>
+        <xdr:cNvPr id="90" name="カギ線コネクタ 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2EBB9A63-2A0C-4FDB-8A1A-623DC9289433}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="14" idx="3"/>
-          <a:endCxn id="117" idx="1"/>
+          <a:stCxn id="73" idx="3"/>
+          <a:endCxn id="75" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22368782" y="11576050"/>
-          <a:ext cx="2316843" cy="3048000"/>
+          <a:off x="23311756" y="18434050"/>
+          <a:ext cx="2469244" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1127579</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1128713</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="62" name="直線矢印コネクタ 61">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0029736-4CC3-4BDD-9F17-458E2B05BEC3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="2"/>
-          <a:endCxn id="110" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="13240204" y="8166100"/>
-          <a:ext cx="1134" cy="2247900"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1127579</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1127579</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="66" name="直線矢印コネクタ 65">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8098FF82-42BA-4FA4-BBE6-730F5E46F03F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="110" idx="2"/>
-          <a:endCxn id="111" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13240204" y="12738100"/>
-          <a:ext cx="0" cy="2247900"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -4039,129 +5020,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:Z45"/>
+  <dimension ref="D1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="P55" sqref="P55"/>
+    <sheetView tabSelected="1" zoomScale="31" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="13.28515625" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:22">
-      <c r="D2" s="3" t="s">
+    <row r="1" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E1" s="4"/>
     </row>
-    <row r="9" spans="4:22">
-      <c r="D9" s="3" t="s">
+    <row r="2" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="8" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="H9" s="3" t="s">
+      <c r="E8" s="4"/>
+      <c r="H8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="L9" s="3" t="s">
+      <c r="I8" s="4"/>
+      <c r="L8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="3"/>
-      <c r="Q9" s="3" t="s">
+      <c r="M8" s="4"/>
+      <c r="Q8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R9" s="3"/>
-      <c r="U9" s="3" t="s">
+      <c r="R8" s="3"/>
+      <c r="U8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="V9" s="3"/>
+      <c r="V8" s="4"/>
     </row>
-    <row r="18" spans="5:26">
-      <c r="L18" s="3" t="s">
+    <row r="9" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="17" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="L17" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="E18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="5:26">
-      <c r="E19" s="3" t="s">
-        <v>4</v>
-      </c>
+    <row r="19" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="21" spans="5:26">
-      <c r="U21" s="2" t="s">
+    <row r="20" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="U20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="V21" s="2"/>
-      <c r="Y21" s="2" t="s">
+      <c r="V20" s="4"/>
+      <c r="Y20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Z21" s="2"/>
+      <c r="Z20" s="4"/>
     </row>
-    <row r="27" spans="5:26">
-      <c r="Q27" s="2" t="s">
+    <row r="21" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+    </row>
+    <row r="26" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="Q26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R27" s="2"/>
+      <c r="R26" s="4"/>
     </row>
-    <row r="35" spans="5:26">
-      <c r="U35" s="2" t="s">
+    <row r="27" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+    </row>
+    <row r="35" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="U35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="V35" s="2"/>
-      <c r="Y35" s="2" t="s">
+      <c r="V35" s="4"/>
+      <c r="Y35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Z35" s="2"/>
+      <c r="Z35" s="4"/>
     </row>
-    <row r="37" spans="5:26">
-      <c r="E37" s="3" t="s">
+    <row r="36" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="E36" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="F36" s="3"/>
+      <c r="K36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+    </row>
+    <row r="37" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
     </row>
-    <row r="39" spans="5:26">
+    <row r="39" spans="5:26" x14ac:dyDescent="0.3">
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
-    <row r="45" spans="5:26">
-      <c r="Q45" s="2" t="s">
+    <row r="44" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="Q44" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R45" s="2"/>
+      <c r="R44" s="4"/>
+      <c r="U44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V44" s="4"/>
+      <c r="Y44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z44" s="4"/>
+    </row>
+    <row r="45" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+    </row>
+    <row r="56" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="I56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="4"/>
+      <c r="O56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P56" s="4"/>
+    </row>
+    <row r="57" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+    </row>
+    <row r="59" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="U59" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V59" s="4"/>
+      <c r="Y59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z59" s="4"/>
+    </row>
+    <row r="60" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="Y60" s="4"/>
+      <c r="Z60" s="4"/>
+    </row>
+    <row r="71" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="U71" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V71" s="4"/>
+    </row>
+    <row r="72" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="I72" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J72" s="4"/>
+      <c r="O72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="P72" s="4"/>
+      <c r="U72" s="4"/>
+      <c r="V72" s="4"/>
+    </row>
+    <row r="73" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+    </row>
+    <row r="81" spans="18:23" x14ac:dyDescent="0.3">
+      <c r="R81" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S81" s="4"/>
+      <c r="V81" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W81" s="4"/>
+    </row>
+    <row r="82" spans="18:23" x14ac:dyDescent="0.3">
+      <c r="R82" s="4"/>
+      <c r="S82" s="4"/>
+      <c r="V82" s="4"/>
+      <c r="W82" s="4"/>
+    </row>
+    <row r="89" spans="18:23" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U89" s="5"/>
+      <c r="V89" s="5"/>
+    </row>
+    <row r="90" spans="18:23" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U90" s="5"/>
+      <c r="V90" s="5"/>
+    </row>
+    <row r="99" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R99" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S99" s="3"/>
+    </row>
+    <row r="100" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R100" s="3"/>
+      <c r="S100" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="L18:M18"/>
+  <mergeCells count="29">
+    <mergeCell ref="Y59:Z60"/>
+    <mergeCell ref="R99:S100"/>
+    <mergeCell ref="R81:S82"/>
+    <mergeCell ref="U71:V72"/>
+    <mergeCell ref="V81:W82"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="Q8:R9"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="Q44:R45"/>
+    <mergeCell ref="Q26:R27"/>
+    <mergeCell ref="O56:P57"/>
+    <mergeCell ref="I56:J57"/>
+    <mergeCell ref="K36:L37"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="L17:M18"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="Y44:Z45"/>
+    <mergeCell ref="O72:P73"/>
+    <mergeCell ref="I72:J73"/>
+    <mergeCell ref="U44:V45"/>
+    <mergeCell ref="U59:V60"/>
+    <mergeCell ref="Y35:Z36"/>
+    <mergeCell ref="U35:V36"/>
+    <mergeCell ref="Y20:Z21"/>
+    <mergeCell ref="U20:V21"/>
     <mergeCell ref="K19:N19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Y35:Z35"/>
   </mergeCells>
-  <phoneticPr fontId="2"/>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>